<commit_message>
Integrated Glen's markdown changes.  Fixed many of the Readme.md files.   Updated the MIDI mapping documentation.   Per Yann request changed 16-channel-volume to 16_channel_volume
</commit_message>
<xml_diff>
--- a/faust-examples/virtualAnalog/MIDI Mappings VA.xlsx
+++ b/faust-examples/virtualAnalog/MIDI Mappings VA.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="99">
   <si>
     <t>White/pink toggle</t>
   </si>
@@ -215,23 +215,140 @@
     <t xml:space="preserve">Glide </t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Sustain</t>
   </si>
   <si>
     <t>midi sustain foot pedal</t>
   </si>
   <si>
-    <t>x 2 keyboard switch -&gt; Knob</t>
+    <t>Master tuning</t>
+  </si>
+  <si>
+    <t>Modulation mix between OSC3 and Noise</t>
+  </si>
+  <si>
+    <t>OSC 1 range</t>
+  </si>
+  <si>
+    <t>OSC 1 detuning</t>
+  </si>
+  <si>
+    <t>OSC 1 waveform shape</t>
+  </si>
+  <si>
+    <t>OSC 2 range</t>
+  </si>
+  <si>
+    <t>OSC 2 detuning</t>
+  </si>
+  <si>
+    <t>OSC 2 waveform shape</t>
+  </si>
+  <si>
+    <t>OSC 3 range</t>
+  </si>
+  <si>
+    <t>OSC 3 detuning</t>
+  </si>
+  <si>
+    <t>OSC 3 waveform shape</t>
+  </si>
+  <si>
+    <t>OSC 3 as a control signal or as an audio source</t>
+  </si>
+  <si>
+    <t>OSC 1 gain</t>
+  </si>
+  <si>
+    <t>OSC 1 enable</t>
+  </si>
+  <si>
+    <t>OSC 2 gain</t>
+  </si>
+  <si>
+    <t>OSC 2 enable</t>
+  </si>
+  <si>
+    <t>OSC 3 gain</t>
+  </si>
+  <si>
+    <t>OSC 3 enable</t>
+  </si>
+  <si>
+    <t>Extrenal input gain</t>
+  </si>
+  <si>
+    <t>External input enable</t>
+  </si>
+  <si>
+    <t>Noise gain</t>
+  </si>
+  <si>
+    <t>Noise Enable</t>
+  </si>
+  <si>
+    <t>Noise pink/white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable modulation control of OSC frequencies </t>
+  </si>
+  <si>
+    <t>Enable modulation control of the filter cutoff frequency</t>
+  </si>
+  <si>
+    <t>Add keyboard control of the filter cutoff frequency</t>
+  </si>
+  <si>
+    <t>Filter cutoff frequency</t>
+  </si>
+  <si>
+    <t>Filter Resonance (Q)</t>
+  </si>
+  <si>
+    <t>Amount of envelope generator</t>
+  </si>
+  <si>
+    <t>VCF envelope generator attack time</t>
+  </si>
+  <si>
+    <t>VCF envelope generator decay time</t>
+  </si>
+  <si>
+    <t>VCF envelope generator sustain level</t>
+  </si>
+  <si>
+    <t>VCA envelope generator attack time</t>
+  </si>
+  <si>
+    <t>VCA envelope generator decay time</t>
+  </si>
+  <si>
+    <t>VCA envelope generator sustain level</t>
+  </si>
+  <si>
+    <t>Enable portamento</t>
+  </si>
+  <si>
+    <t>Modulation Wheel control</t>
+  </si>
+  <si>
+    <t>Master volume</t>
+  </si>
+  <si>
+    <t>Portamento time</t>
+  </si>
+  <si>
+    <t>Enables using the decay stage as a release stage</t>
+  </si>
+  <si>
+    <t>Note sustain, preempts the VCF/VCA release stage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -270,8 +387,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,8 +420,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -506,8 +648,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="207">
+  <cellStyleXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -715,35 +870,90 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="207">
+  <cellStyles count="235">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -847,6 +1057,20 @@
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -950,6 +1174,20 @@
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1289,815 +1527,819 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E53" sqref="A5:E53"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="31.1640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="18" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="16" thickBot="1"/>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>47</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" thickBot="1">
+      <c r="A8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="11">
+        <v>48</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" thickBot="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:5" ht="28">
+      <c r="A10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="7">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="9">
+        <v>23</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9">
+        <v>24</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="9">
+        <v>25</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="9">
+        <v>28</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="9">
+        <v>29</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="9">
+        <v>30</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="9">
+        <v>33</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="9">
+        <v>34</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="9">
+        <v>35</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" thickBot="1">
+      <c r="A20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="11">
+        <v>9</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" thickBot="1">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="23"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="7">
+        <v>26</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" thickBot="1">
+      <c r="A23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="9">
+        <v>12</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="9">
+        <v>31</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" thickBot="1">
+      <c r="A25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="9">
+        <v>14</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="9">
+        <v>36</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="9">
+        <v>17</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="9">
+        <v>27</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="9">
+        <v>13</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="9">
+        <v>32</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="9">
+        <v>15</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" thickBot="1">
+      <c r="A32" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="11">
+        <v>16</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="23"/>
+    </row>
+    <row r="34" spans="1:5" ht="28">
+      <c r="A34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="9">
+        <v>19</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28">
+      <c r="A35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="9">
+        <v>38</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="9">
+        <v>74</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="9">
+        <v>37</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="9">
+        <v>39</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="28">
+      <c r="A39" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="9">
+        <v>40</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="28">
+      <c r="A40" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="9">
+        <v>41</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29" thickBot="1">
+      <c r="A41" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="11">
+        <v>42</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="16" thickBot="1">
+      <c r="A42" s="12"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="1:5" ht="28">
+      <c r="A43" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="7">
+        <v>43</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="28">
+      <c r="A44" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="9">
+        <v>44</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29" thickBot="1">
+      <c r="A45" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="11">
+        <v>45</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16" thickBot="1">
+      <c r="A46" s="12"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="23"/>
+    </row>
+    <row r="47" spans="1:5" ht="28">
+      <c r="A47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="7">
+        <v>20</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="9">
+        <v>65</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="29" thickBot="1">
+      <c r="A51" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="11">
-        <v>5</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1">
-      <c r="A8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="14">
-        <v>48</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" thickBot="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="8">
-        <v>22</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="B51" s="11">
+        <v>64</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="11">
-        <v>23</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="11">
-        <v>24</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="11">
-        <v>25</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="11">
-        <v>28</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="10" t="s">
+      <c r="E51" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="16" thickBot="1">
+      <c r="A52" s="12"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="23"/>
+    </row>
+    <row r="53" spans="1:5" ht="16" thickBot="1">
+      <c r="A53" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="16">
         <v>7</v>
       </c>
-      <c r="B15" s="11">
-        <v>29</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="11">
-        <v>30</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="11">
-        <v>33</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="11">
-        <v>34</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="11">
-        <v>35</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" thickBot="1">
-      <c r="A20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="14">
-        <v>9</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16" thickBot="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="22"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="8">
+      <c r="C53" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="11">
-        <v>12</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="11">
-        <v>31</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="11">
-        <v>14</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="11">
-        <v>36</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="11">
-        <v>17</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="11">
-        <v>27</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="11">
-        <v>13</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="11">
-        <v>32</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="11">
-        <v>15</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="16" thickBot="1">
-      <c r="A32" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="14">
-        <v>16</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="21"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="22"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="11">
-        <v>19</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="11">
-        <v>38</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="11">
-        <v>74</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="11">
-        <v>37</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="11">
-        <v>39</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="11">
-        <v>40</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="11">
-        <v>41</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="16" thickBot="1">
-      <c r="A41" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="14">
-        <v>42</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="16" thickBot="1">
-      <c r="A42" s="21"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="22"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="8">
-        <v>43</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="11">
-        <v>44</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="16" thickBot="1">
-      <c r="A45" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="14">
-        <v>45</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="16" thickBot="1">
-      <c r="A46" s="21"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="22"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" s="8">
-        <v>20</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="11">
-        <v>65</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="12"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="11">
-        <v>1</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="16" thickBot="1">
-      <c r="A51" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" s="14">
-        <v>64</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" s="15"/>
-    </row>
-    <row r="52" spans="1:5" ht="16" thickBot="1">
-      <c r="A52" s="21"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="22"/>
-    </row>
-    <row r="53" spans="1:5" ht="16" thickBot="1">
-      <c r="A53" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="18">
-        <v>7</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>56</v>
+      <c r="D53" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>